<commit_message>
Update Dataset Basic Example
</commit_message>
<xml_diff>
--- a/jupyter_notebooks/file/input/basic_example_tim/network.xlsx
+++ b/jupyter_notebooks/file/input/basic_example_tim/network.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mn6461\Documents\GitHub\reXplan-repo\jupyter_notebooks\file\input\basic_example_tim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5D52445-00E8-4F6A-AC48-76F0EBC7BB28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4AB03D7-76A1-41C3-9843-AC0ED71127E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="-8940" windowWidth="25440" windowHeight="15390" firstSheet="3" activeTab="8" xr2:uid="{9ECEC293-7360-4DDE-9C10-8A2C51BA16DF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="8" xr2:uid="{9ECEC293-7360-4DDE-9C10-8A2C51BA16DF}"/>
   </bookViews>
   <sheets>
     <sheet name="simulation" sheetId="12" r:id="rId1"/>
@@ -22,8 +22,8 @@
     <sheet name="tr_type" sheetId="6" r:id="rId7"/>
     <sheet name="transformers" sheetId="3" r:id="rId8"/>
     <sheet name="lines" sheetId="4" r:id="rId9"/>
-    <sheet name="switches" sheetId="14" r:id="rId10"/>
-    <sheet name="ln_type" sheetId="7" r:id="rId11"/>
+    <sheet name="ln_type" sheetId="7" r:id="rId10"/>
+    <sheet name="switches" sheetId="14" r:id="rId11"/>
     <sheet name="cost" sheetId="10" r:id="rId12"/>
     <sheet name="profiles" sheetId="11" r:id="rId13"/>
     <sheet name="crews" sheetId="13" r:id="rId14"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="178">
   <si>
     <t>name</t>
   </si>
@@ -539,9 +539,6 @@
     <t>lineSpan</t>
   </si>
   <si>
-    <t>0.2</t>
-  </si>
-  <si>
     <t>element</t>
   </si>
   <si>
@@ -576,6 +573,15 @@
   </si>
   <si>
     <t>False</t>
+  </si>
+  <si>
+    <t>rp3</t>
+  </si>
+  <si>
+    <t>pole_type_1</t>
+  </si>
+  <si>
+    <t>pole_type_2</t>
   </si>
 </sst>
 </file>
@@ -651,7 +657,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Gut" xfId="1" builtinId="26"/>
@@ -1013,103 +1019,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F048EE5-6CF5-4D91-BE31-E59CF33F6687}">
-  <dimension ref="A1:I11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="40" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.88671875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" t="s">
-        <v>164</v>
-      </c>
-      <c r="D1" t="s">
-        <v>165</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" t="s">
-        <v>166</v>
-      </c>
-      <c r="G1" t="s">
-        <v>167</v>
-      </c>
-      <c r="H1" t="s">
-        <v>168</v>
-      </c>
-      <c r="I1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G2" s="2"/>
-      <c r="I2" s="2"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G4" s="2"/>
-      <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B643028-F04F-4526-8B5B-4E99E7FCEC09}">
   <dimension ref="A1:K2"/>
   <sheetViews>
@@ -1185,6 +1094,103 @@
       <c r="K2" t="s">
         <v>46</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F048EE5-6CF5-4D91-BE31-E59CF33F6687}">
+  <dimension ref="A1:I11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="40" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>165</v>
+      </c>
+      <c r="G1" t="s">
+        <v>166</v>
+      </c>
+      <c r="H1" t="s">
+        <v>167</v>
+      </c>
+      <c r="I1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G2" s="2"/>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G4" s="2"/>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4782,7 +4788,7 @@
   <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:E19"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5678,7 +5684,7 @@
         <v>158</v>
       </c>
       <c r="AA1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.3">
@@ -5701,7 +5707,7 @@
         <v>105</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="X2" s="2"/>
       <c r="Z2">
@@ -5728,7 +5734,7 @@
         <v>105</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="X3" s="2"/>
       <c r="Z3">
@@ -5755,7 +5761,7 @@
         <v>105</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="X4" s="2"/>
       <c r="Z4">
@@ -5782,7 +5788,7 @@
         <v>105</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="X5" s="2"/>
       <c r="Z5">
@@ -5809,7 +5815,7 @@
         <v>105</v>
       </c>
       <c r="V6" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="X6" s="2"/>
       <c r="Z6">
@@ -5836,7 +5842,7 @@
         <v>105</v>
       </c>
       <c r="V7" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="X7" s="2"/>
       <c r="Z7">
@@ -5967,7 +5973,7 @@
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6100,7 +6106,7 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6156,7 +6162,7 @@
         <v>158</v>
       </c>
       <c r="M1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -6192,694 +6198,694 @@
   <dimension ref="A1:S17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="1.88671875" customWidth="1"/>
-    <col min="11" max="11" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.33203125" customWidth="1"/>
-    <col min="14" max="14" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.21875" customWidth="1"/>
+    <col min="9" max="9" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="16" width="1.88671875" customWidth="1"/>
+    <col min="17" max="17" width="4.33203125" customWidth="1"/>
+    <col min="18" max="18" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>30</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>31</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>32</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>162</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" t="s">
+        <v>101</v>
+      </c>
+      <c r="K1" t="s">
+        <v>169</v>
+      </c>
+      <c r="L1" t="s">
+        <v>158</v>
+      </c>
+      <c r="M1" t="s">
+        <v>70</v>
+      </c>
+      <c r="N1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O1" t="s">
+        <v>69</v>
+      </c>
+      <c r="P1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>35</v>
+      </c>
+      <c r="F2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2">
+        <v>0.2</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I2">
+        <v>100</v>
+      </c>
+      <c r="J2" t="s">
+        <v>172</v>
+      </c>
+      <c r="K2" t="s">
+        <v>175</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3">
+        <v>25</v>
+      </c>
+      <c r="F3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3">
+        <v>0.2</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I3">
+        <v>100</v>
+      </c>
+      <c r="J3" t="s">
+        <v>172</v>
+      </c>
+      <c r="K3" t="s">
+        <v>175</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>106</v>
+      </c>
+      <c r="E4">
+        <v>20.5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4">
+        <v>0.2</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I4">
+        <v>100</v>
+      </c>
+      <c r="J4" t="s">
+        <v>172</v>
+      </c>
+      <c r="K4" t="s">
+        <v>171</v>
+      </c>
+      <c r="L4" s="6">
+        <v>3</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D5" t="s">
+        <v>107</v>
+      </c>
+      <c r="E5">
+        <v>21</v>
+      </c>
+      <c r="F5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5">
+        <v>0.2</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I5">
+        <v>100</v>
+      </c>
+      <c r="J5" t="s">
+        <v>176</v>
+      </c>
+      <c r="K5" t="s">
+        <v>171</v>
+      </c>
+      <c r="L5">
+        <v>3</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>120</v>
+      </c>
+      <c r="C6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D6" t="s">
+        <v>108</v>
+      </c>
+      <c r="E6">
+        <v>21.5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6">
+        <v>0.2</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I6">
+        <v>100</v>
+      </c>
+      <c r="J6" t="s">
+        <v>173</v>
+      </c>
+      <c r="K6" t="s">
+        <v>171</v>
+      </c>
+      <c r="L6">
+        <v>3</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>121</v>
+      </c>
+      <c r="C7" t="s">
+        <v>108</v>
+      </c>
+      <c r="D7" t="s">
+        <v>109</v>
+      </c>
+      <c r="E7">
+        <v>22</v>
+      </c>
+      <c r="F7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7">
+        <v>0.2</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I7">
+        <v>100</v>
+      </c>
+      <c r="J7" t="s">
+        <v>173</v>
+      </c>
+      <c r="K7" t="s">
+        <v>171</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D8" t="s">
+        <v>110</v>
+      </c>
+      <c r="E8">
+        <v>22.5</v>
+      </c>
+      <c r="F8" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8">
+        <v>0.2</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I8">
+        <v>100</v>
+      </c>
+      <c r="J8" t="s">
+        <v>176</v>
+      </c>
+      <c r="K8" t="s">
+        <v>170</v>
+      </c>
+      <c r="L8">
+        <v>2</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>123</v>
+      </c>
+      <c r="C9" t="s">
+        <v>109</v>
+      </c>
+      <c r="D9" t="s">
+        <v>133</v>
+      </c>
+      <c r="E9">
+        <v>23</v>
+      </c>
+      <c r="F9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9">
+        <v>0.2</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I9">
+        <v>100</v>
+      </c>
+      <c r="J9" t="s">
+        <v>176</v>
+      </c>
+      <c r="K9" t="s">
+        <v>171</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>124</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>111</v>
+      </c>
+      <c r="E10">
+        <v>23.5</v>
+      </c>
+      <c r="F10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10">
+        <v>0.2</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I10">
+        <v>100</v>
+      </c>
+      <c r="J10" t="s">
+        <v>172</v>
+      </c>
+      <c r="K10" t="s">
+        <v>175</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="R10" s="7"/>
+      <c r="S10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C11" t="s">
+        <v>111</v>
+      </c>
+      <c r="D11" t="s">
+        <v>112</v>
+      </c>
+      <c r="E11">
+        <v>24</v>
+      </c>
+      <c r="F11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G11">
+        <v>0.2</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I11">
+        <v>100</v>
+      </c>
+      <c r="J11" t="s">
+        <v>173</v>
+      </c>
+      <c r="K11" t="s">
+        <v>175</v>
+      </c>
+      <c r="L11">
+        <v>3</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>126</v>
+      </c>
+      <c r="C12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D12" t="s">
+        <v>113</v>
+      </c>
+      <c r="E12">
+        <v>24.5</v>
+      </c>
+      <c r="F12" t="s">
+        <v>45</v>
+      </c>
+      <c r="G12">
+        <v>0.2</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I12">
+        <v>100</v>
+      </c>
+      <c r="J12" t="s">
+        <v>173</v>
+      </c>
+      <c r="K12" t="s">
+        <v>170</v>
+      </c>
+      <c r="L12">
+        <v>3</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>127</v>
+      </c>
+      <c r="C13" t="s">
+        <v>113</v>
+      </c>
+      <c r="D13" t="s">
+        <v>114</v>
+      </c>
+      <c r="E13">
+        <v>25</v>
+      </c>
+      <c r="F13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13">
+        <v>0.2</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I13">
+        <v>100</v>
+      </c>
+      <c r="J13" t="s">
+        <v>173</v>
+      </c>
+      <c r="K13" t="s">
+        <v>170</v>
+      </c>
+      <c r="L13">
+        <v>3</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>128</v>
+      </c>
+      <c r="C14" t="s">
+        <v>114</v>
+      </c>
+      <c r="D14" t="s">
+        <v>115</v>
+      </c>
+      <c r="E14">
+        <v>25.5</v>
+      </c>
+      <c r="F14" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14">
+        <v>0.2</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I14">
+        <v>100</v>
+      </c>
+      <c r="J14" t="s">
+        <v>177</v>
+      </c>
+      <c r="K14" t="s">
+        <v>170</v>
+      </c>
+      <c r="L14">
+        <v>4</v>
+      </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>129</v>
+      </c>
+      <c r="C15" t="s">
+        <v>114</v>
+      </c>
+      <c r="D15" t="s">
+        <v>116</v>
+      </c>
+      <c r="E15">
+        <v>26</v>
+      </c>
+      <c r="F15" t="s">
+        <v>45</v>
+      </c>
+      <c r="G15">
+        <v>0.2</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I15">
+        <v>100</v>
+      </c>
+      <c r="J15" t="s">
+        <v>173</v>
+      </c>
+      <c r="K15" t="s">
+        <v>170</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>130</v>
+      </c>
+      <c r="C16" t="s">
+        <v>116</v>
+      </c>
+      <c r="D16" t="s">
+        <v>117</v>
+      </c>
+      <c r="E16">
+        <v>26.5</v>
+      </c>
+      <c r="F16" t="s">
+        <v>45</v>
+      </c>
+      <c r="G16">
+        <v>0.2</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I16">
+        <v>100</v>
+      </c>
+      <c r="J16" t="s">
+        <v>177</v>
+      </c>
+      <c r="K16" t="s">
+        <v>170</v>
+      </c>
+      <c r="L16">
+        <v>2</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>131</v>
+      </c>
+      <c r="C17" t="s">
+        <v>116</v>
+      </c>
+      <c r="D17" t="s">
+        <v>132</v>
+      </c>
+      <c r="E17">
         <v>27</v>
       </c>
-      <c r="G1" t="s">
-        <v>70</v>
-      </c>
-      <c r="H1" t="s">
-        <v>67</v>
-      </c>
-      <c r="I1" t="s">
-        <v>69</v>
-      </c>
-      <c r="J1" t="s">
-        <v>68</v>
-      </c>
-      <c r="K1" t="s">
-        <v>101</v>
-      </c>
-      <c r="L1" t="s">
-        <v>3</v>
-      </c>
-      <c r="M1" t="s">
-        <v>33</v>
-      </c>
-      <c r="N1" t="s">
-        <v>34</v>
-      </c>
-      <c r="O1" t="s">
-        <v>35</v>
-      </c>
-      <c r="P1" t="s">
-        <v>157</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>158</v>
-      </c>
-      <c r="R1" t="s">
-        <v>162</v>
-      </c>
-      <c r="S1" t="s">
+      <c r="F17" t="s">
+        <v>45</v>
+      </c>
+      <c r="G17">
+        <v>0.2</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I17">
+        <v>100</v>
+      </c>
+      <c r="J17" t="s">
+        <v>177</v>
+      </c>
+      <c r="K17" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2">
-        <v>35</v>
-      </c>
-      <c r="E2" t="s">
-        <v>45</v>
-      </c>
-      <c r="K2" t="s">
-        <v>173</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="O2">
-        <v>100</v>
-      </c>
-      <c r="P2">
+      <c r="L17">
+        <v>2</v>
+      </c>
+      <c r="S17">
         <v>0</v>
-      </c>
-      <c r="Q2">
-        <v>1</v>
-      </c>
-      <c r="R2" t="s">
-        <v>163</v>
-      </c>
-      <c r="S2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3">
-        <v>25</v>
-      </c>
-      <c r="E3" t="s">
-        <v>45</v>
-      </c>
-      <c r="K3" t="s">
-        <v>173</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="O3">
-        <v>100</v>
-      </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
-      <c r="Q3">
-        <v>4</v>
-      </c>
-      <c r="R3" t="s">
-        <v>163</v>
-      </c>
-      <c r="S3" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>118</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>106</v>
-      </c>
-      <c r="D4">
-        <v>20.5</v>
-      </c>
-      <c r="E4" t="s">
-        <v>45</v>
-      </c>
-      <c r="K4" t="s">
-        <v>174</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="O4">
-        <v>100</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="6">
-        <v>3</v>
-      </c>
-      <c r="R4" t="s">
-        <v>163</v>
-      </c>
-      <c r="S4" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>119</v>
-      </c>
-      <c r="B5" t="s">
-        <v>106</v>
-      </c>
-      <c r="C5" t="s">
-        <v>107</v>
-      </c>
-      <c r="D5">
-        <v>21</v>
-      </c>
-      <c r="E5" t="s">
-        <v>45</v>
-      </c>
-      <c r="K5" t="s">
-        <v>173</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="O5">
-        <v>100</v>
-      </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
-      <c r="Q5">
-        <v>3</v>
-      </c>
-      <c r="R5" t="s">
-        <v>163</v>
-      </c>
-      <c r="S5" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>120</v>
-      </c>
-      <c r="B6" t="s">
-        <v>106</v>
-      </c>
-      <c r="C6" t="s">
-        <v>108</v>
-      </c>
-      <c r="D6">
-        <v>21.5</v>
-      </c>
-      <c r="E6" t="s">
-        <v>45</v>
-      </c>
-      <c r="K6" t="s">
-        <v>173</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="O6">
-        <v>100</v>
-      </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-      <c r="Q6">
-        <v>3</v>
-      </c>
-      <c r="R6" t="s">
-        <v>163</v>
-      </c>
-      <c r="S6" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>121</v>
-      </c>
-      <c r="B7" t="s">
-        <v>108</v>
-      </c>
-      <c r="C7" t="s">
-        <v>109</v>
-      </c>
-      <c r="D7">
-        <v>22</v>
-      </c>
-      <c r="E7" t="s">
-        <v>45</v>
-      </c>
-      <c r="K7" t="s">
-        <v>174</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="O7">
-        <v>100</v>
-      </c>
-      <c r="P7">
-        <v>0</v>
-      </c>
-      <c r="Q7">
-        <v>1</v>
-      </c>
-      <c r="R7" t="s">
-        <v>163</v>
-      </c>
-      <c r="S7" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>122</v>
-      </c>
-      <c r="B8" t="s">
-        <v>109</v>
-      </c>
-      <c r="C8" t="s">
-        <v>110</v>
-      </c>
-      <c r="D8">
-        <v>22.5</v>
-      </c>
-      <c r="E8" t="s">
-        <v>45</v>
-      </c>
-      <c r="K8" t="s">
-        <v>174</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="O8">
-        <v>100</v>
-      </c>
-      <c r="P8">
-        <v>0</v>
-      </c>
-      <c r="Q8">
-        <v>2</v>
-      </c>
-      <c r="R8" t="s">
-        <v>163</v>
-      </c>
-      <c r="S8" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>123</v>
-      </c>
-      <c r="B9" t="s">
-        <v>109</v>
-      </c>
-      <c r="C9" t="s">
-        <v>133</v>
-      </c>
-      <c r="D9">
-        <v>23</v>
-      </c>
-      <c r="E9" t="s">
-        <v>45</v>
-      </c>
-      <c r="K9" t="s">
-        <v>174</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="O9">
-        <v>100</v>
-      </c>
-      <c r="P9">
-        <v>0</v>
-      </c>
-      <c r="Q9">
-        <v>1</v>
-      </c>
-      <c r="R9" t="s">
-        <v>163</v>
-      </c>
-      <c r="S9" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>124</v>
-      </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" t="s">
-        <v>111</v>
-      </c>
-      <c r="D10">
-        <v>23.5</v>
-      </c>
-      <c r="E10" t="s">
-        <v>45</v>
-      </c>
-      <c r="K10" t="s">
-        <v>173</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="N10" s="7"/>
-      <c r="O10">
-        <v>100</v>
-      </c>
-      <c r="P10">
-        <v>0</v>
-      </c>
-      <c r="Q10">
-        <v>1</v>
-      </c>
-      <c r="R10" t="s">
-        <v>163</v>
-      </c>
-      <c r="S10" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>125</v>
-      </c>
-      <c r="B11" t="s">
-        <v>111</v>
-      </c>
-      <c r="C11" t="s">
-        <v>112</v>
-      </c>
-      <c r="D11">
-        <v>24</v>
-      </c>
-      <c r="E11" t="s">
-        <v>45</v>
-      </c>
-      <c r="K11" t="s">
-        <v>174</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="O11">
-        <v>100</v>
-      </c>
-      <c r="P11">
-        <v>0</v>
-      </c>
-      <c r="Q11">
-        <v>0</v>
-      </c>
-      <c r="R11" t="s">
-        <v>163</v>
-      </c>
-      <c r="S11" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>126</v>
-      </c>
-      <c r="B12" t="s">
-        <v>111</v>
-      </c>
-      <c r="C12" t="s">
-        <v>113</v>
-      </c>
-      <c r="D12">
-        <v>24.5</v>
-      </c>
-      <c r="E12" t="s">
-        <v>45</v>
-      </c>
-      <c r="K12" t="s">
-        <v>173</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="O12">
-        <v>100</v>
-      </c>
-      <c r="P12">
-        <v>0</v>
-      </c>
-      <c r="Q12">
-        <v>3</v>
-      </c>
-      <c r="R12" t="s">
-        <v>163</v>
-      </c>
-      <c r="S12" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>127</v>
-      </c>
-      <c r="B13" t="s">
-        <v>113</v>
-      </c>
-      <c r="C13" t="s">
-        <v>114</v>
-      </c>
-      <c r="D13">
-        <v>25</v>
-      </c>
-      <c r="E13" t="s">
-        <v>45</v>
-      </c>
-      <c r="K13" t="s">
-        <v>173</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="O13">
-        <v>100</v>
-      </c>
-      <c r="P13">
-        <v>0</v>
-      </c>
-      <c r="Q13">
-        <v>3</v>
-      </c>
-      <c r="R13" t="s">
-        <v>163</v>
-      </c>
-      <c r="S13" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>128</v>
-      </c>
-      <c r="B14" t="s">
-        <v>114</v>
-      </c>
-      <c r="C14" t="s">
-        <v>115</v>
-      </c>
-      <c r="D14">
-        <v>25.5</v>
-      </c>
-      <c r="E14" t="s">
-        <v>45</v>
-      </c>
-      <c r="K14" t="s">
-        <v>174</v>
-      </c>
-      <c r="L14" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="O14">
-        <v>100</v>
-      </c>
-      <c r="P14">
-        <v>0</v>
-      </c>
-      <c r="Q14">
-        <v>4</v>
-      </c>
-      <c r="R14" t="s">
-        <v>163</v>
-      </c>
-      <c r="S14" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>129</v>
-      </c>
-      <c r="B15" t="s">
-        <v>114</v>
-      </c>
-      <c r="C15" t="s">
-        <v>116</v>
-      </c>
-      <c r="D15">
-        <v>26</v>
-      </c>
-      <c r="E15" t="s">
-        <v>45</v>
-      </c>
-      <c r="K15" t="s">
-        <v>174</v>
-      </c>
-      <c r="L15" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="O15">
-        <v>100</v>
-      </c>
-      <c r="P15">
-        <v>0</v>
-      </c>
-      <c r="Q15">
-        <v>1</v>
-      </c>
-      <c r="R15" t="s">
-        <v>163</v>
-      </c>
-      <c r="S15" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>130</v>
-      </c>
-      <c r="B16" t="s">
-        <v>116</v>
-      </c>
-      <c r="C16" t="s">
-        <v>117</v>
-      </c>
-      <c r="D16">
-        <v>26.5</v>
-      </c>
-      <c r="E16" t="s">
-        <v>45</v>
-      </c>
-      <c r="K16" t="s">
-        <v>174</v>
-      </c>
-      <c r="L16" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="O16">
-        <v>100</v>
-      </c>
-      <c r="P16">
-        <v>0</v>
-      </c>
-      <c r="Q16">
-        <v>0</v>
-      </c>
-      <c r="R16" t="s">
-        <v>163</v>
-      </c>
-      <c r="S16" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>131</v>
-      </c>
-      <c r="B17" t="s">
-        <v>116</v>
-      </c>
-      <c r="C17" t="s">
-        <v>132</v>
-      </c>
-      <c r="D17">
-        <v>27</v>
-      </c>
-      <c r="E17" t="s">
-        <v>45</v>
-      </c>
-      <c r="K17" t="s">
-        <v>174</v>
-      </c>
-      <c r="L17" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="O17">
-        <v>100</v>
-      </c>
-      <c r="P17">
-        <v>0</v>
-      </c>
-      <c r="Q17">
-        <v>2</v>
-      </c>
-      <c r="R17" t="s">
-        <v>163</v>
-      </c>
-      <c r="S17" t="s">
-        <v>172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>